<commit_message>
rest of sample data
</commit_message>
<xml_diff>
--- a/raw_data/final_samples/SVSHW_infaunal_sept2020.xlsx
+++ b/raw_data/final_samples/SVSHW_infaunal_sept2020.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Amelia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Amelia/Documents/UBC/R_projects/SVSHW_2020/raw_data/final_samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88741DD9-D36C-3146-A4C9-9AF470A004BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BCBCF7-D889-D445-9F78-BBB46A192451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{8C231DDD-7964-684B-A131-20C8A477D24E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="42">
   <si>
     <t>block</t>
   </si>
@@ -136,6 +136,30 @@
   </si>
   <si>
     <t>onchidoris_bliamellata</t>
+  </si>
+  <si>
+    <t>emplectonema_gracile</t>
+  </si>
+  <si>
+    <t>pagurus_hirsutiusculus</t>
+  </si>
+  <si>
+    <t>limpet_recruit</t>
+  </si>
+  <si>
+    <t>grey, short</t>
+  </si>
+  <si>
+    <t>polychaeta_2</t>
+  </si>
+  <si>
+    <t>oedoperna_larvae</t>
+  </si>
+  <si>
+    <t>insecta_2</t>
+  </si>
+  <si>
+    <t>tick</t>
   </si>
 </sst>
 </file>
@@ -487,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE5BA77-F3F6-B741-BF77-4E83BDB2AB7E}">
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L133" sqref="L133"/>
+      <selection activeCell="G176" sqref="G176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2459,6 +2483,586 @@
         <v>1</v>
       </c>
     </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>15</v>
+      </c>
+      <c r="B140">
+        <v>6</v>
+      </c>
+      <c r="C140" t="s">
+        <v>14</v>
+      </c>
+      <c r="D140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>15</v>
+      </c>
+      <c r="B141">
+        <v>6</v>
+      </c>
+      <c r="C141" t="s">
+        <v>22</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>15</v>
+      </c>
+      <c r="B142">
+        <v>6</v>
+      </c>
+      <c r="C142" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>15</v>
+      </c>
+      <c r="B143">
+        <v>6</v>
+      </c>
+      <c r="C143" t="s">
+        <v>10</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>13</v>
+      </c>
+      <c r="B144">
+        <v>16</v>
+      </c>
+      <c r="C144" t="s">
+        <v>19</v>
+      </c>
+      <c r="D144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>13</v>
+      </c>
+      <c r="B145">
+        <v>16</v>
+      </c>
+      <c r="C145" t="s">
+        <v>22</v>
+      </c>
+      <c r="D145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>13</v>
+      </c>
+      <c r="B146">
+        <v>16</v>
+      </c>
+      <c r="C146" t="s">
+        <v>12</v>
+      </c>
+      <c r="D146">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>13</v>
+      </c>
+      <c r="B147">
+        <v>16</v>
+      </c>
+      <c r="C147" t="s">
+        <v>14</v>
+      </c>
+      <c r="D147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>13</v>
+      </c>
+      <c r="B148">
+        <v>16</v>
+      </c>
+      <c r="C148" t="s">
+        <v>10</v>
+      </c>
+      <c r="D148">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>13</v>
+      </c>
+      <c r="B149">
+        <v>16</v>
+      </c>
+      <c r="C149" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>23</v>
+      </c>
+      <c r="B150">
+        <v>15</v>
+      </c>
+      <c r="C150" t="s">
+        <v>19</v>
+      </c>
+      <c r="D150">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>23</v>
+      </c>
+      <c r="B151">
+        <v>15</v>
+      </c>
+      <c r="C151" t="s">
+        <v>22</v>
+      </c>
+      <c r="D151">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>23</v>
+      </c>
+      <c r="B152">
+        <v>15</v>
+      </c>
+      <c r="C152" t="s">
+        <v>18</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>23</v>
+      </c>
+      <c r="B153">
+        <v>15</v>
+      </c>
+      <c r="C153" t="s">
+        <v>34</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>23</v>
+      </c>
+      <c r="B154">
+        <v>15</v>
+      </c>
+      <c r="C154" t="s">
+        <v>14</v>
+      </c>
+      <c r="D154">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>23</v>
+      </c>
+      <c r="B155">
+        <v>15</v>
+      </c>
+      <c r="C155" t="s">
+        <v>35</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>23</v>
+      </c>
+      <c r="B156">
+        <v>15</v>
+      </c>
+      <c r="C156" t="s">
+        <v>10</v>
+      </c>
+      <c r="D156">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>23</v>
+      </c>
+      <c r="B157">
+        <v>15</v>
+      </c>
+      <c r="C157" t="s">
+        <v>24</v>
+      </c>
+      <c r="D157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>23</v>
+      </c>
+      <c r="B158">
+        <v>15</v>
+      </c>
+      <c r="C158" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>23</v>
+      </c>
+      <c r="B159">
+        <v>15</v>
+      </c>
+      <c r="C159" t="s">
+        <v>26</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>23</v>
+      </c>
+      <c r="B160">
+        <v>15</v>
+      </c>
+      <c r="C160" t="s">
+        <v>12</v>
+      </c>
+      <c r="D160">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>23</v>
+      </c>
+      <c r="B161">
+        <v>15</v>
+      </c>
+      <c r="C161" t="s">
+        <v>36</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>2</v>
+      </c>
+      <c r="B162">
+        <v>4</v>
+      </c>
+      <c r="C162" t="s">
+        <v>19</v>
+      </c>
+      <c r="D162">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>2</v>
+      </c>
+      <c r="B163">
+        <v>4</v>
+      </c>
+      <c r="C163" t="s">
+        <v>22</v>
+      </c>
+      <c r="D163">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>2</v>
+      </c>
+      <c r="B164">
+        <v>4</v>
+      </c>
+      <c r="C164" t="s">
+        <v>14</v>
+      </c>
+      <c r="D164">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>2</v>
+      </c>
+      <c r="B165">
+        <v>4</v>
+      </c>
+      <c r="C165" t="s">
+        <v>34</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>2</v>
+      </c>
+      <c r="B166">
+        <v>4</v>
+      </c>
+      <c r="C166" t="s">
+        <v>26</v>
+      </c>
+      <c r="D166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>2</v>
+      </c>
+      <c r="B167">
+        <v>4</v>
+      </c>
+      <c r="C167" t="s">
+        <v>24</v>
+      </c>
+      <c r="D167">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>2</v>
+      </c>
+      <c r="B168">
+        <v>4</v>
+      </c>
+      <c r="C168" t="s">
+        <v>12</v>
+      </c>
+      <c r="D168">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>2</v>
+      </c>
+      <c r="B169">
+        <v>4</v>
+      </c>
+      <c r="C169" t="s">
+        <v>10</v>
+      </c>
+      <c r="D169">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>2</v>
+      </c>
+      <c r="B170">
+        <v>4</v>
+      </c>
+      <c r="C170" t="s">
+        <v>6</v>
+      </c>
+      <c r="D170">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>2</v>
+      </c>
+      <c r="B171">
+        <v>4</v>
+      </c>
+      <c r="C171" t="s">
+        <v>30</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>23</v>
+      </c>
+      <c r="B172">
+        <v>6</v>
+      </c>
+      <c r="C172" t="s">
+        <v>19</v>
+      </c>
+      <c r="D172">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>23</v>
+      </c>
+      <c r="B173">
+        <v>6</v>
+      </c>
+      <c r="C173" t="s">
+        <v>22</v>
+      </c>
+      <c r="D173">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>23</v>
+      </c>
+      <c r="B174">
+        <v>6</v>
+      </c>
+      <c r="C174" t="s">
+        <v>38</v>
+      </c>
+      <c r="D174">
+        <v>2</v>
+      </c>
+      <c r="E174" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>23</v>
+      </c>
+      <c r="B175">
+        <v>6</v>
+      </c>
+      <c r="C175" t="s">
+        <v>14</v>
+      </c>
+      <c r="D175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>23</v>
+      </c>
+      <c r="B176">
+        <v>6</v>
+      </c>
+      <c r="C176" t="s">
+        <v>12</v>
+      </c>
+      <c r="D176">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>23</v>
+      </c>
+      <c r="B177">
+        <v>6</v>
+      </c>
+      <c r="C177" t="s">
+        <v>10</v>
+      </c>
+      <c r="D177">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>23</v>
+      </c>
+      <c r="B178">
+        <v>6</v>
+      </c>
+      <c r="C178" t="s">
+        <v>6</v>
+      </c>
+      <c r="D178">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>23</v>
+      </c>
+      <c r="B179">
+        <v>6</v>
+      </c>
+      <c r="C179" t="s">
+        <v>39</v>
+      </c>
+      <c r="D179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>23</v>
+      </c>
+      <c r="B180">
+        <v>6</v>
+      </c>
+      <c r="C180" t="s">
+        <v>40</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+      <c r="E180" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
it's been a long time
</commit_message>
<xml_diff>
--- a/raw_data/final_samples/SVSHW_infaunal_sept2020.xlsx
+++ b/raw_data/final_samples/SVSHW_infaunal_sept2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Amelia/Documents/UBC/R_projects/SVSHW_2020/raw_data/final_samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BCBCF7-D889-D445-9F78-BBB46A192451}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BF5CC1-2F30-BE40-82CA-4637469161CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{8C231DDD-7964-684B-A131-20C8A477D24E}"/>
   </bookViews>
@@ -514,7 +514,7 @@
   <dimension ref="A1:E180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G176" sqref="G176"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,7 +967,7 @@
         <v>11</v>
       </c>
       <c r="B32">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
@@ -981,7 +981,7 @@
         <v>11</v>
       </c>
       <c r="B33">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -995,7 +995,7 @@
         <v>11</v>
       </c>
       <c r="B34">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
@@ -1009,7 +1009,7 @@
         <v>11</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -1026,7 +1026,7 @@
         <v>11</v>
       </c>
       <c r="B36">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C36" t="s">
         <v>22</v>

</xml_diff>